<commit_message>
Reorg of static data
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data_2.0/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data_2.0/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWILKE06\Documents\Eclipse_Repos\metroceri\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data_2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F940E3F9-0513-4DDA-A40D-68266A809361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923F4F08-3493-4355-9595-87336A029275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28950" yWindow="30" windowWidth="11055" windowHeight="15570" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-28920" yWindow="1230" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="379">
   <si>
     <t>ID</t>
   </si>
@@ -1134,6 +1134,48 @@
   </si>
   <si>
     <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>InteractiveActivity</t>
+  </si>
+  <si>
+    <t>Wordcloud</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>Noteboard Activity</t>
+  </si>
+  <si>
+    <t>ERBInnerPanel</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>Project Creation</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Not in content.xml</t>
   </si>
 </sst>
 </file>
@@ -3779,8 +3821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AD5C8-E087-42D9-8818-93A09826D8C4}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5358,20 +5400,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="78.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="83" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="83" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
@@ -5381,8 +5424,11 @@
       <c r="C1" s="83" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="83" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="76" t="s">
         <v>59</v>
       </c>
@@ -5393,7 +5439,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="76" t="s">
         <v>60</v>
       </c>
@@ -5404,7 +5450,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="76" t="s">
         <v>61</v>
       </c>
@@ -5415,7 +5461,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="76" t="s">
         <v>62</v>
       </c>
@@ -5426,7 +5472,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="76" t="s">
         <v>63</v>
       </c>
@@ -5437,7 +5483,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="76" t="s">
         <v>64</v>
       </c>
@@ -5448,7 +5494,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="76" t="s">
         <v>65</v>
       </c>
@@ -5459,7 +5505,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="76" t="s">
         <v>263</v>
       </c>
@@ -5470,7 +5516,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="76" t="s">
         <v>265</v>
       </c>
@@ -5481,7 +5527,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="76" t="s">
         <v>152</v>
       </c>
@@ -5492,7 +5538,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="76" t="s">
         <v>157</v>
       </c>
@@ -5503,7 +5549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="76" t="s">
         <v>158</v>
       </c>
@@ -5514,7 +5560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="76" t="s">
         <v>159</v>
       </c>
@@ -5525,7 +5571,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="76" t="s">
         <v>160</v>
       </c>
@@ -5536,7 +5582,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="76" t="s">
         <v>268</v>
       </c>
@@ -6251,7 +6297,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="76" t="s">
         <v>359</v>
       </c>
@@ -6262,7 +6308,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="76" t="s">
         <v>361</v>
       </c>
@@ -6273,7 +6319,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="76" t="s">
         <v>363</v>
       </c>
@@ -6284,7 +6330,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="76" t="s">
         <v>364</v>
       </c>
@@ -6293,6 +6339,104 @@
       </c>
       <c r="C84" t="s">
         <v>234</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="76" t="s">
+        <v>365</v>
+      </c>
+      <c r="B85" t="s">
+        <v>366</v>
+      </c>
+      <c r="C85" t="s">
+        <v>367</v>
+      </c>
+      <c r="D85" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="76" t="s">
+        <v>368</v>
+      </c>
+      <c r="B86" t="s">
+        <v>366</v>
+      </c>
+      <c r="C86" t="s">
+        <v>369</v>
+      </c>
+      <c r="D86" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="76" t="s">
+        <v>371</v>
+      </c>
+      <c r="B87" t="s">
+        <v>370</v>
+      </c>
+      <c r="C87" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="D87" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="76" t="s">
+        <v>372</v>
+      </c>
+      <c r="B88" t="s">
+        <v>370</v>
+      </c>
+      <c r="C88" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D88" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="76" t="s">
+        <v>373</v>
+      </c>
+      <c r="B89" t="s">
+        <v>370</v>
+      </c>
+      <c r="C89" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="76" t="s">
+        <v>374</v>
+      </c>
+      <c r="B90" t="s">
+        <v>370</v>
+      </c>
+      <c r="C90" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="D90" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="76" t="s">
+        <v>375</v>
+      </c>
+      <c r="B91" t="s">
+        <v>370</v>
+      </c>
+      <c r="C91" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="D91" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code to read goal categories
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data_2.0/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data_2.0/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWILKE06\Documents\Eclipse_Repos\metroceri\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data_2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923F4F08-3493-4355-9595-87336A029275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D965A7-BF6F-4A4E-BE9D-8A09ADE364AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1230" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="29595" yWindow="0" windowWidth="11460" windowHeight="15585" firstSheet="1" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="379">
   <si>
     <t>ID</t>
   </si>
@@ -3821,8 +3821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AD5C8-E087-42D9-8818-93A09826D8C4}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4562,8 +4562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C403D9B-4156-4D53-B432-05D214EB9E6F}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5402,8 +5402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6351,9 +6351,6 @@
       <c r="C85" t="s">
         <v>367</v>
       </c>
-      <c r="D85" t="s">
-        <v>378</v>
-      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="76" t="s">
@@ -6364,9 +6361,6 @@
       </c>
       <c r="C86" t="s">
         <v>369</v>
-      </c>
-      <c r="D86" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>